<commit_message>
tdf#141309 tdf#142215 OOXML import: fix double conversion in autofilter
resulting missing selection of filtered time values
and numbers ending with zeroes.

No need to convert the filter values from string to
number and back at OOXML import, because we'll do that later
in the model by filtering with the formatted cell values.

Follow-up to commit 31d94710d07de8812bcc33ca7363250d7d17cd95
"Related: tdf#140968 avoid duplicated filter values".

Change-Id: I75e5b2391624ff85a8ed545926ec519355a356bc
Reviewed-on: https://gerrit.libreoffice.org/c/core/+/115473
Tested-by: László Németh <nemeth@numbertext.org>
Reviewed-by: László Németh <nemeth@numbertext.org>
</commit_message>
<xml_diff>
--- a/sc/qa/uitest/data/autofilter/tdf140968.xlsx
+++ b/sc/qa/uitest/data/autofilter/tdf140968.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Munka1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Munka1!$A$1:$B$7</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Munka1!$A$1:$B$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t xml:space="preserve">Values</t>
   </si>
@@ -120,15 +120,15 @@
       <charset val="238"/>
     </font>
     <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -312,11 +312,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -386,15 +386,15 @@
     <cellStyle name="Error 9" xfId="25"/>
     <cellStyle name="Footnote 10" xfId="26"/>
     <cellStyle name="Good 11" xfId="27"/>
-    <cellStyle name="Heading" xfId="28"/>
-    <cellStyle name="Heading 1 13" xfId="29"/>
-    <cellStyle name="Heading 12" xfId="30"/>
-    <cellStyle name="Heading 2 14" xfId="31"/>
+    <cellStyle name="Heading 1 13" xfId="28"/>
+    <cellStyle name="Heading 12" xfId="29"/>
+    <cellStyle name="Heading 2 14" xfId="30"/>
+    <cellStyle name="Heading 3" xfId="31"/>
     <cellStyle name="Hyperlink 15" xfId="32"/>
     <cellStyle name="Neutral 16" xfId="33"/>
     <cellStyle name="Note 17" xfId="34"/>
-    <cellStyle name="Result" xfId="35"/>
-    <cellStyle name="Result 18" xfId="36"/>
+    <cellStyle name="Result 18" xfId="35"/>
+    <cellStyle name="Result 4" xfId="36"/>
     <cellStyle name="Status 19" xfId="37"/>
     <cellStyle name="Text 20" xfId="38"/>
     <cellStyle name="Warning 21" xfId="39"/>
@@ -471,19 +471,19 @@
   <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="2" style="0" width="8.72"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -491,7 +491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0.364849537037037</v>
       </c>
@@ -499,7 +499,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>0.0458680555555556</v>
       </c>
@@ -507,7 +507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>0.0458796296296296</v>
       </c>
@@ -515,7 +515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>0.0458912037037037</v>
       </c>
@@ -523,7 +523,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>0</v>
       </c>
@@ -531,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>0.516030092592593</v>
       </c>
@@ -539,11 +539,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B7">
+  <autoFilter ref="A1:B8">
     <filterColumn colId="0">
       <filters>
         <filter val="0.046"/>
+        <filter val="0.500"/>
         <filter val="0.516"/>
       </filters>
     </filterColumn>

</xml_diff>